<commit_message>
add readme; improve import script
</commit_message>
<xml_diff>
--- a/CreateEmployees/employees.xlsx
+++ b/CreateEmployees/employees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\powershell\CreateEmployees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381DAF70-38B9-4FFF-B27E-E865171A94E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED387490-028D-4D7A-B9D1-494888507D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8190" yWindow="780" windowWidth="26520" windowHeight="14970" xr2:uid="{B4A8875B-A54E-425B-93A0-E5772367BD29}"/>
+    <workbookView xWindow="4770" yWindow="555" windowWidth="31680" windowHeight="14970" xr2:uid="{B4A8875B-A54E-425B-93A0-E5772367BD29}"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -312,9 +312,6 @@
     <t>512-6100-5000 x12334</t>
   </si>
   <si>
-    <t xml:space="preserve">Mr. </t>
-  </si>
-  <si>
     <t>Dr</t>
   </si>
   <si>
@@ -322,6 +319,12 @@
   </si>
   <si>
     <t>Calamity</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Mr</t>
   </si>
 </sst>
 </file>
@@ -886,7 +889,7 @@
   <dimension ref="A1:AO5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,16 +1105,16 @@
         <v>50</v>
       </c>
       <c r="O2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P2" t="s">
         <v>82</v>
       </c>
       <c r="Q2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="R2" t="s">
+        <v>46</v>
       </c>
       <c r="S2" t="s">
         <v>80</v>
@@ -1235,8 +1238,8 @@
       <c r="Q3" t="s">
         <v>45</v>
       </c>
-      <c r="R3" t="b">
-        <v>1</v>
+      <c r="R3" t="s">
+        <v>46</v>
       </c>
       <c r="S3" t="s">
         <v>80</v>
@@ -1358,10 +1361,10 @@
         <v>84</v>
       </c>
       <c r="Q4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" t="s">
         <v>94</v>
-      </c>
-      <c r="R4" t="b">
-        <v>0</v>
       </c>
       <c r="S4" t="s">
         <v>80</v>
@@ -1477,7 +1480,7 @@
         <v>50</v>
       </c>
       <c r="O5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="P5" t="s">
         <v>85</v>
@@ -1485,8 +1488,8 @@
       <c r="Q5" t="s">
         <v>45</v>
       </c>
-      <c r="R5" t="b">
-        <v>1</v>
+      <c r="R5" t="s">
+        <v>46</v>
       </c>
       <c r="S5" t="s">
         <v>80</v>

</xml_diff>